<commit_message>
Continue with EDX UT and UCSD (on-time graded) and Udacity Inferential Stats
</commit_message>
<xml_diff>
--- a/Stats/Udacity/DataAnalystNanoDegree/IntroToInferentialStats/Lesson10_Regression.xlsx
+++ b/Stats/Udacity/DataAnalystNanoDegree/IntroToInferentialStats/Lesson10_Regression.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NEWNSS\Dropbox\DataScienceMasters\Stats\Udacity\DataAnalystNanoDegree\IntroToInferentialStats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nimz\Dropbox\DataScienceMasters\Stats\Udacity\DataAnalystNanoDegree\IntroToInferentialStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="planes" sheetId="1" r:id="rId1"/>
     <sheet name="problem set" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>r</t>
   </si>
@@ -150,17 +150,26 @@
     <t>expected alcoholic beverages due to caffeine beverages</t>
   </si>
   <si>
-    <t>SE</t>
+    <t>CI (estimated +/- SE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r2 </t>
+  </si>
+  <si>
+    <t>&lt;-- 20% of the variation in alcoholic beverages is likely caused by/due to variation in caffeinated beverages/is related to caffeinated beverages</t>
+  </si>
+  <si>
+    <t>SE of the estimate (n/sqrt(sd)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +223,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -314,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -345,6 +363,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -369,19 +400,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -669,25 +691,25 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="5.28515625" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" customWidth="1"/>
+    <col min="11" max="11" width="5.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -713,7 +735,7 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>337</v>
       </c>
@@ -728,10 +750,10 @@
         <f>PEARSON(A2:A10,B2:B10)</f>
         <v>0.9090036493537198</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="18"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="10"/>
@@ -746,7 +768,7 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2565</v>
       </c>
@@ -761,13 +783,13 @@
         <f>_xlfn.STDEV.S(A2:A10)</f>
         <v>2315.3368245486681</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="13"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="18"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -779,7 +801,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>967</v>
       </c>
@@ -794,13 +816,13 @@
         <f>_xlfn.STDEV.S(B2:B10)</f>
         <v>508.18700228798099</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="13"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="18"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -812,7 +834,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>5124</v>
       </c>
@@ -843,7 +865,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>2398</v>
       </c>
@@ -876,7 +898,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>2586</v>
       </c>
@@ -907,7 +929,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7412</v>
       </c>
@@ -938,7 +960,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>522</v>
       </c>
@@ -969,7 +991,7 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>1499</v>
       </c>
@@ -984,24 +1006,24 @@
         <f>E8-E5*E7</f>
         <v>161.38775380144136</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="15"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="20"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="4"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
@@ -1023,7 +1045,7 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
@@ -1045,28 +1067,28 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-    </row>
-    <row r="13" spans="1:30" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q12" s="22"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+    </row>
+    <row r="13" spans="1:30" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
       <c r="D13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="12">
         <f>4000*E5+E10</f>
         <v>959.44673983937855</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="9">
         <f>E5</f>
         <v>0.19951474650948431</v>
@@ -1079,22 +1101,22 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="18"/>
-      <c r="AD13" s="18"/>
-    </row>
-    <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q13" s="22"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+      <c r="X13" s="23"/>
+      <c r="Y13" s="23"/>
+      <c r="Z13" s="23"/>
+      <c r="AA13" s="23"/>
+      <c r="AB13" s="23"/>
+      <c r="AC13" s="23"/>
+      <c r="AD13" s="23"/>
+    </row>
+    <row r="14" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
@@ -1114,7 +1136,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
@@ -1138,7 +1160,7 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
@@ -1162,7 +1184,7 @@
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
@@ -1189,7 +1211,7 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
@@ -1211,7 +1233,7 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
     </row>
-    <row r="19" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
@@ -1233,7 +1255,7 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
     </row>
-    <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1259,7 +1281,7 @@
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
     </row>
-    <row r="21" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -1285,7 +1307,7 @@
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
     </row>
-    <row r="22" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1311,7 +1333,7 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
     </row>
-    <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
@@ -1337,7 +1359,7 @@
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
     </row>
-    <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1366,13 +1388,13 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
     </row>
-    <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
+    <row r="25" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="23"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1390,7 +1412,7 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
     </row>
-    <row r="26" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
@@ -1412,7 +1434,7 @@
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
     </row>
-    <row r="27" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
@@ -1434,7 +1456,7 @@
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
     </row>
-    <row r="28" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
@@ -1456,7 +1478,7 @@
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
     </row>
-    <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
@@ -1478,7 +1500,7 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
     </row>
-    <row r="30" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
@@ -1500,7 +1522,7 @@
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
     </row>
-    <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
@@ -1522,7 +1544,7 @@
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
     </row>
-    <row r="32" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="3"/>
@@ -1544,7 +1566,7 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
     </row>
-    <row r="33" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
@@ -1566,7 +1588,7 @@
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
     </row>
-    <row r="34" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="3"/>
@@ -1588,7 +1610,7 @@
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
     </row>
-    <row r="35" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="3"/>
@@ -1610,7 +1632,7 @@
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
     </row>
-    <row r="36" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="3"/>
@@ -1632,7 +1654,7 @@
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
     </row>
-    <row r="37" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="3"/>
@@ -1654,7 +1676,7 @@
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
     </row>
-    <row r="38" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="3"/>
@@ -1676,7 +1698,7 @@
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
     </row>
-    <row r="39" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
@@ -1698,7 +1720,7 @@
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
     </row>
-    <row r="40" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
@@ -1720,7 +1742,7 @@
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
     </row>
-    <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="3"/>
@@ -1742,7 +1764,7 @@
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
     </row>
-    <row r="42" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
@@ -1764,7 +1786,7 @@
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
     </row>
-    <row r="43" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
@@ -1786,7 +1808,7 @@
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
     </row>
-    <row r="44" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="3"/>
@@ -1808,7 +1830,7 @@
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
     </row>
-    <row r="45" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="3"/>
@@ -1830,7 +1852,7 @@
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
     </row>
-    <row r="46" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="3"/>
@@ -1852,7 +1874,7 @@
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
     </row>
-    <row r="47" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="3"/>
@@ -1874,7 +1896,7 @@
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
     </row>
-    <row r="48" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
@@ -1896,7 +1918,7 @@
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
     </row>
-    <row r="49" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="3"/>
@@ -1918,7 +1940,7 @@
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
     </row>
-    <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="3"/>
@@ -1940,7 +1962,7 @@
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
     </row>
-    <row r="51" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="3"/>
@@ -1962,7 +1984,7 @@
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
     </row>
-    <row r="52" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
@@ -1984,7 +2006,7 @@
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
     </row>
-    <row r="53" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="3"/>
@@ -2006,7 +2028,7 @@
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
     </row>
-    <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="3"/>
@@ -2028,7 +2050,7 @@
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
     </row>
-    <row r="55" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="3"/>
@@ -2050,7 +2072,7 @@
       <c r="S55" s="2"/>
       <c r="T55" s="2"/>
     </row>
-    <row r="56" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="3"/>
@@ -2072,7 +2094,7 @@
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
     </row>
-    <row r="57" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="3"/>
@@ -2094,7 +2116,7 @@
       <c r="S57" s="2"/>
       <c r="T57" s="2"/>
     </row>
-    <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="3"/>
@@ -2116,7 +2138,7 @@
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
     </row>
-    <row r="59" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="3"/>
@@ -2138,7 +2160,7 @@
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
     </row>
-    <row r="60" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="3"/>
@@ -2160,7 +2182,7 @@
       <c r="S60" s="2"/>
       <c r="T60" s="2"/>
     </row>
-    <row r="61" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="3"/>
@@ -2182,7 +2204,7 @@
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
     </row>
-    <row r="62" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="3"/>
@@ -2204,7 +2226,7 @@
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
     </row>
-    <row r="63" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2226,7 +2248,7 @@
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
     </row>
-    <row r="64" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2248,7 +2270,7 @@
       <c r="S64" s="2"/>
       <c r="T64" s="2"/>
     </row>
-    <row r="65" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2270,7 +2292,7 @@
       <c r="S65" s="2"/>
       <c r="T65" s="2"/>
     </row>
-    <row r="66" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2292,7 +2314,7 @@
       <c r="S66" s="2"/>
       <c r="T66" s="2"/>
     </row>
-    <row r="67" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2314,7 +2336,7 @@
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
     </row>
-    <row r="68" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2336,7 +2358,7 @@
       <c r="S68" s="2"/>
       <c r="T68" s="2"/>
     </row>
-    <row r="69" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2358,7 +2380,7 @@
       <c r="S69" s="2"/>
       <c r="T69" s="2"/>
     </row>
-    <row r="70" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2380,7 +2402,7 @@
       <c r="S70" s="2"/>
       <c r="T70" s="2"/>
     </row>
-    <row r="71" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2402,7 +2424,7 @@
       <c r="S71" s="2"/>
       <c r="T71" s="2"/>
     </row>
-    <row r="72" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2424,7 +2446,7 @@
       <c r="S72" s="2"/>
       <c r="T72" s="2"/>
     </row>
-    <row r="73" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2446,7 +2468,7 @@
       <c r="S73" s="2"/>
       <c r="T73" s="2"/>
     </row>
-    <row r="74" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2468,7 +2490,7 @@
       <c r="S74" s="2"/>
       <c r="T74" s="2"/>
     </row>
-    <row r="75" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2490,7 +2512,7 @@
       <c r="S75" s="2"/>
       <c r="T75" s="2"/>
     </row>
-    <row r="76" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2512,7 +2534,7 @@
       <c r="S76" s="2"/>
       <c r="T76" s="2"/>
     </row>
-    <row r="77" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2534,7 +2556,7 @@
       <c r="S77" s="2"/>
       <c r="T77" s="2"/>
     </row>
-    <row r="78" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2556,7 +2578,7 @@
       <c r="S78" s="2"/>
       <c r="T78" s="2"/>
     </row>
-    <row r="79" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2578,7 +2600,7 @@
       <c r="S79" s="2"/>
       <c r="T79" s="2"/>
     </row>
-    <row r="80" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2600,7 +2622,7 @@
       <c r="S80" s="2"/>
       <c r="T80" s="2"/>
     </row>
-    <row r="81" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2622,7 +2644,7 @@
       <c r="S81" s="2"/>
       <c r="T81" s="2"/>
     </row>
-    <row r="82" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2644,7 +2666,7 @@
       <c r="S82" s="2"/>
       <c r="T82" s="2"/>
     </row>
-    <row r="83" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2666,7 +2688,7 @@
       <c r="S83" s="2"/>
       <c r="T83" s="2"/>
     </row>
-    <row r="84" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2688,7 +2710,7 @@
       <c r="S84" s="2"/>
       <c r="T84" s="2"/>
     </row>
-    <row r="85" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2710,7 +2732,7 @@
       <c r="S85" s="2"/>
       <c r="T85" s="2"/>
     </row>
-    <row r="86" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2732,7 +2754,7 @@
       <c r="S86" s="2"/>
       <c r="T86" s="2"/>
     </row>
-    <row r="87" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2754,7 +2776,7 @@
       <c r="S87" s="2"/>
       <c r="T87" s="2"/>
     </row>
-    <row r="88" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2776,7 +2798,7 @@
       <c r="S88" s="2"/>
       <c r="T88" s="2"/>
     </row>
-    <row r="89" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2798,7 +2820,7 @@
       <c r="S89" s="2"/>
       <c r="T89" s="2"/>
     </row>
-    <row r="90" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2820,7 +2842,7 @@
       <c r="S90" s="2"/>
       <c r="T90" s="2"/>
     </row>
-    <row r="91" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2842,7 +2864,7 @@
       <c r="S91" s="2"/>
       <c r="T91" s="2"/>
     </row>
-    <row r="92" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2864,7 +2886,7 @@
       <c r="S92" s="2"/>
       <c r="T92" s="2"/>
     </row>
-    <row r="93" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2886,7 +2908,7 @@
       <c r="S93" s="2"/>
       <c r="T93" s="2"/>
     </row>
-    <row r="94" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2908,7 +2930,7 @@
       <c r="S94" s="2"/>
       <c r="T94" s="2"/>
     </row>
-    <row r="95" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2930,7 +2952,7 @@
       <c r="S95" s="2"/>
       <c r="T95" s="2"/>
     </row>
-    <row r="96" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2952,7 +2974,7 @@
       <c r="S96" s="2"/>
       <c r="T96" s="2"/>
     </row>
-    <row r="97" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2974,7 +2996,7 @@
       <c r="S97" s="2"/>
       <c r="T97" s="2"/>
     </row>
-    <row r="98" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2996,7 +3018,7 @@
       <c r="S98" s="2"/>
       <c r="T98" s="2"/>
     </row>
-    <row r="99" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3018,7 +3040,7 @@
       <c r="S99" s="2"/>
       <c r="T99" s="2"/>
     </row>
-    <row r="100" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -3058,21 +3080,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -3080,7 +3102,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>116</v>
       </c>
@@ -3088,7 +3110,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>117</v>
       </c>
@@ -3103,7 +3125,7 @@
         <v>0.93446503062490205</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>120</v>
       </c>
@@ -3118,7 +3140,7 @@
         <v>38.258892523736975</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -3133,7 +3155,7 @@
         <v>23.429123106164464</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>52</v>
       </c>
@@ -3148,7 +3170,7 @@
         <v>0.5722511760457536</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>79</v>
       </c>
@@ -3166,7 +3188,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>109</v>
       </c>
@@ -3181,7 +3203,7 @@
         <v>70.8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>27</v>
       </c>
@@ -3196,7 +3218,7 @@
         <v>38.266666666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>85</v>
       </c>
@@ -3211,7 +3233,7 @@
         <v>-2.2487165973726846</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>51</v>
       </c>
@@ -3226,7 +3248,7 @@
         <v>0.572251176045754x + -2.24871659737268</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>78</v>
       </c>
@@ -3235,7 +3257,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>55</v>
       </c>
@@ -3246,7 +3268,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>26</v>
       </c>
@@ -3258,7 +3280,7 @@
         <v>126.25350479244125</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>39</v>
       </c>
@@ -3266,7 +3288,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>107</v>
       </c>
@@ -3277,21 +3299,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="24">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="13">
         <f>(0-E10)/E6</f>
         <v>3.9295971620561447</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -3299,7 +3321,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -3310,60 +3332,119 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
         <v>10</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <f>B25*$B$24+$B$23</f>
         <v>2.85</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
         <v>5</v>
       </c>
-      <c r="C26">
-        <f t="shared" ref="C26:C29" si="0">B26*$B$24+$B$23</f>
+      <c r="C26" s="1">
+        <f>B26*$B$24+$B$23</f>
         <v>2.6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
         <v>0</v>
       </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
+      <c r="C27" s="1">
+        <f t="shared" ref="C26:C28" si="0">B27*$B$24+$B$23</f>
         <v>2.35</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="1">
         <v>20</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <f t="shared" si="0"/>
         <v>3.35</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:4" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B29">
-        <v>3.5</v>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="1">
+        <f>C25-$B$30</f>
+        <v>-0.64999999999999991</v>
+      </c>
+      <c r="C32" s="1">
+        <f>C25+$B$30</f>
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="1">
+        <f>C26-$B$30</f>
+        <v>-0.89999999999999991</v>
+      </c>
+      <c r="C33" s="1">
+        <f>C26+$B$30</f>
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="1">
+        <f>C27-$B$30</f>
+        <v>-1.1499999999999999</v>
+      </c>
+      <c r="C34" s="1">
+        <f>C27+$B$30</f>
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="1">
+        <f>C28-$B$30</f>
+        <v>-0.14999999999999991</v>
+      </c>
+      <c r="C35" s="1">
+        <f>C28+$B$30</f>
+        <v>6.85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37">
+        <v>0.2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>